<commit_message>
Update on DB connect
</commit_message>
<xml_diff>
--- a/Resources/support.xlsx
+++ b/Resources/support.xlsx
@@ -399,7 +399,7 @@
       <selection activeCell="B3" sqref="B3:B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
     <col width="6.81640625" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="11.90625" customWidth="1" min="2" max="2"/>
@@ -3401,7 +3401,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
     <col width="52" customWidth="1" min="1" max="1"/>
   </cols>
@@ -3488,15 +3488,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col width="5.36328125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="40" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="6" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="32" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3577,6 +3580,160 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>'No Cost Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TylerLarson@rep.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>400463</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>'No Cost Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>StephanieLynn@rep.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>400465</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>'No Cost Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TinaJohnson@rep.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>400466</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>'No Cost Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MaryJoyce@rep.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>400470</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>'30$ kit Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MichaelFisher@rep.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>400472</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>'30$ kit Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GeorgeKeller@rep.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>400478</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>'30$ kit Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>StacyJenkins@rep.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>400479</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>'No Cost Signup'</t>
         </is>

</xml_diff>

<commit_message>
API & DB patch
</commit_message>
<xml_diff>
--- a/Resources/support.xlsx
+++ b/Resources/support.xlsx
@@ -3396,7 +3396,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView zoomScale="76" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -3693,6 +3693,342 @@
       <c r="B24" t="inlineStr">
         <is>
           <t>AVC2109150159844</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>100091365</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>AVR2109160159882</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>100091366</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>AVC2109160159884</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>100091368</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>AVC2109160159888</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>100091371</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>AVR2109160159892</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>100091373</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>AVR2109160159895</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>100091379</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>AVC2109160159911</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>100091380</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>AVC2109160159912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>100091381</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>AVC2109160159913</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>100091382</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>AVC2109160159914</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>100091383</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>AVC2109160159915</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>100091385</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>AVC2109160159922</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>100091386</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>AVC2109160159923</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>100091387</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>AVC2109160159924</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>100091388</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>AVR2109160159925</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>100091390</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>AVR2109160159930</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>100091391</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>AVR2109160159933</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>100091392</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>AVR2109160159935</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>100091393</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>AVR2109160159937</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>100091394</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>AVR2109160159939</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>100091395</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>AVR2109160159941</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>100091396</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>AVR2109160159943</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>100091397</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>AVR2109160159945</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>100091399</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>AVR2109160159951</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>100091401</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>AVR2109160159955</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>100091403</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>AVR2109160159962</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>100091412</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>AVR2109160159993</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>100091413</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>AVR2109160159995</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>100091414</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>AVR2109160159997</t>
         </is>
       </c>
     </row>
@@ -3801,18 +4137,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col width="54" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="62" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="6" customWidth="1" min="2" max="2"/>
     <col width="12" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="32" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5286,6 +5622,408 @@
       <c r="D72" t="inlineStr">
         <is>
           <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>PS_KimberlySteele890355@rep.com</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>400780</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>'No Cost Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>PS_LarryCooper438458@rep.com</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>400781</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>'No Cost Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>PS_CarlWillis987884@rep.com</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>400782</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>'Donation Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>PS_DianeStark251159@rep.com</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>400783</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>'30$ kit Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>PS_MatthewDalton830636@cust.com</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Attached</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>PS_DouglasHale299767@cust.com</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>PS_JeremyJones818349@rep.com</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>400788</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>'Donation Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>PS_ShaunThomas345399@rep.com</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>400789</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>'30$ kit Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>PS_MelindaSingh531223@rep.com</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>400791</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>'30$ kit Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>PS_TanyaLawson263831@cust.com</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>PS_TonyaMoore484276@cust.com</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>PS_ReneeRiley097838@cust.com</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>PS_StevenWagner596338@cust.com</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>PS_BrendaLevine471513@cust.com</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>PS_TiffanyWaters591843@cust.com</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>PS_JustinParks532136@cust.com</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>PS_MarkMerritt066755@cust.com</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>PS_LaurenDay052291@cust.com</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>PS_AndreHoffman032937@cust.com</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Cust</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Unattached</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>PS_AlanHarris521913@rep.com</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>400804</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>'30$ kit Signup'</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>PS_AndrewStafford029758@rep.com</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>REP</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>400806</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>'30$ kit Signup'</t>
         </is>
       </c>
     </row>

</xml_diff>